<commit_message>
added another data provider and a new test case
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="Register" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>mohit</t>
   </si>
@@ -32,6 +33,21 @@
   </si>
   <si>
     <t>david</t>
+  </si>
+  <si>
+    <t>rock</t>
+  </si>
+  <si>
+    <t>baby</t>
+  </si>
+  <si>
+    <t>justine</t>
+  </si>
+  <si>
+    <t>biber</t>
+  </si>
+  <si>
+    <t>rat</t>
   </si>
 </sst>
 </file>
@@ -67,8 +83,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,8 +392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,4 +428,57 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1">
+        <v>8870034785</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3223445666</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1">
+        <v>12112122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added data provider to read data from excel
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="Register" sheetId="2" r:id="rId2"/>
+    <sheet name="searchTermList" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>mohit</t>
   </si>
@@ -48,12 +49,27 @@
   </si>
   <si>
     <t>rat</t>
+  </si>
+  <si>
+    <t>hats</t>
+  </si>
+  <si>
+    <t>sofa</t>
+  </si>
+  <si>
+    <t>long dress</t>
+  </si>
+  <si>
+    <t>rings</t>
+  </si>
+  <si>
+    <t>watches</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -434,7 +450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -481,4 +497,44 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>